<commit_message>
20240623 项目名称修改(X-Station -> Sparrow)
</commit_message>
<xml_diff>
--- a/doc/mqtt通信topic.xlsx
+++ b/doc/mqtt通信topic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16425" windowHeight="27495"/>
+    <workbookView windowHeight="17655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>由于免费服务器允许的最大topic个数为10个，为了利用有限的资源，数据采用JSON格式保存和传递，即一个topic保存一组JSON数据。</t>
   </si>
@@ -108,6 +108,14 @@
     <t>设备led灯控制
 0:不开启led
 1:开启led</t>
+  </si>
+  <si>
+    <t>"tools_token"</t>
+  </si>
+  <si>
+    <t>手机令牌功能
+0:关闭手机令牌
+1:开启手机令牌</t>
   </si>
   <si>
     <t>/settings/app_config/disretained</t>
@@ -967,7 +975,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1021,12 +1029,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1571,7 +1573,7 @@
   <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:G9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1715,13 +1717,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" ht="40.5" spans="2:7">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
+      <c r="E9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="12"/>
@@ -1729,7 +1737,7 @@
       <c r="D10" s="16"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="12"/>
@@ -1737,7 +1745,7 @@
       <c r="D11" s="16"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="20"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="12"/>
@@ -1745,7 +1753,7 @@
       <c r="D12" s="16"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="12"/>
@@ -1753,7 +1761,7 @@
       <c r="D13" s="16"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="12"/>
@@ -1761,7 +1769,7 @@
       <c r="D14" s="16"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
-      <c r="G14" s="20"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="12"/>
@@ -1769,7 +1777,7 @@
       <c r="D15" s="16"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="12"/>
@@ -1777,7 +1785,7 @@
       <c r="D16" s="16"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="20"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="12"/>
@@ -1785,7 +1793,7 @@
       <c r="D17" s="16"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="12"/>
@@ -1793,37 +1801,37 @@
       <c r="D18" s="16"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="20"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="21"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="20"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" ht="27" spans="1:7">
       <c r="A20" s="1">
         <v>2</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D20" s="12">
         <v>1</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -1831,13 +1839,13 @@
       <c r="C21" s="13"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="20" t="s">
-        <v>29</v>
+      <c r="G21" s="18" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -1846,7 +1854,7 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="20"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="12"/>
@@ -1854,7 +1862,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
-      <c r="G23" s="20"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="12"/>
@@ -1862,7 +1870,7 @@
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="20"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="12"/>
@@ -1870,7 +1878,7 @@
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
-      <c r="G25" s="20"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="12"/>
@@ -1878,7 +1886,7 @@
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="20"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7">
       <c r="B27" s="12"/>
@@ -1886,7 +1894,7 @@
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="20"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7">
       <c r="B28" s="12"/>
@@ -1894,7 +1902,7 @@
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
-      <c r="G28" s="20"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7">
       <c r="B29" s="12"/>
@@ -1902,7 +1910,7 @@
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
-      <c r="G29" s="20"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7">
       <c r="B30" s="12"/>
@@ -1910,7 +1918,7 @@
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
-      <c r="G30" s="20"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7">
       <c r="B31" s="12"/>
@@ -1918,24 +1926,24 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
-      <c r="G31" s="20"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>3</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D32" s="12">
         <v>1</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
-      <c r="G32" s="20"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="12"/>
@@ -1943,7 +1951,7 @@
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
-      <c r="G33" s="20"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="12"/>
@@ -1951,7 +1959,7 @@
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
-      <c r="G34" s="20"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="12"/>
@@ -1959,7 +1967,7 @@
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
-      <c r="G35" s="20"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7">
       <c r="B36" s="12"/>
@@ -1967,7 +1975,7 @@
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
-      <c r="G36" s="20"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="12"/>
@@ -1975,7 +1983,7 @@
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
-      <c r="G37" s="20"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="12"/>
@@ -1983,7 +1991,7 @@
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
-      <c r="G38" s="20"/>
+      <c r="G38" s="18"/>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="12"/>
@@ -1991,24 +1999,24 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
-      <c r="G39" s="20"/>
+      <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>4</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D40" s="12">
         <v>1</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
-      <c r="G40" s="20"/>
+      <c r="G40" s="18"/>
     </row>
     <row r="41" spans="2:7">
       <c r="B41" s="12"/>
@@ -2016,7 +2024,7 @@
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
-      <c r="G41" s="20"/>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" s="12"/>
@@ -2024,7 +2032,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
-      <c r="G42" s="20"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="2:7">
       <c r="B43" s="12"/>
@@ -2032,7 +2040,7 @@
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
-      <c r="G43" s="20"/>
+      <c r="G43" s="18"/>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" s="12"/>
@@ -2040,7 +2048,7 @@
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
-      <c r="G44" s="20"/>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="2:7">
       <c r="B45" s="12"/>
@@ -2048,7 +2056,7 @@
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
-      <c r="G45" s="20"/>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="2:7">
       <c r="B46" s="12"/>
@@ -2056,7 +2064,7 @@
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
-      <c r="G46" s="20"/>
+      <c r="G46" s="18"/>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="12"/>
@@ -2064,7 +2072,7 @@
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
-      <c r="G47" s="20"/>
+      <c r="G47" s="18"/>
     </row>
     <row r="48" spans="2:7">
       <c r="B48" s="12"/>
@@ -2072,7 +2080,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
-      <c r="G48" s="20"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7">
       <c r="B49" s="12"/>
@@ -2080,215 +2088,215 @@
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
-      <c r="G49" s="20"/>
+      <c r="G49" s="18"/>
     </row>
     <row r="50" ht="81" spans="1:7">
       <c r="A50" s="1">
         <v>5</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="D50" s="14">
         <v>1</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="2:7">
       <c r="B51" s="16"/>
-      <c r="C51" s="23"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="16"/>
       <c r="E51" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F51" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="2:7">
       <c r="B52" s="16"/>
-      <c r="C52" s="23"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="16"/>
       <c r="E52" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G52" s="20" t="s">
-        <v>41</v>
+      <c r="G52" s="18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="2:7">
       <c r="B53" s="16"/>
-      <c r="C53" s="23"/>
+      <c r="C53" s="21"/>
       <c r="D53" s="16"/>
       <c r="E53" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G53" s="20" t="s">
-        <v>43</v>
+      <c r="G53" s="18" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="16"/>
-      <c r="C54" s="23"/>
+      <c r="C54" s="21"/>
       <c r="D54" s="16"/>
       <c r="E54" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G54" s="20" t="s">
-        <v>45</v>
+      <c r="G54" s="18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="2:7">
       <c r="B55" s="16"/>
-      <c r="C55" s="23"/>
+      <c r="C55" s="21"/>
       <c r="D55" s="16"/>
       <c r="E55" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G55" s="20" t="s">
-        <v>47</v>
+      <c r="G55" s="18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="2:7">
       <c r="B56" s="16"/>
-      <c r="C56" s="23"/>
+      <c r="C56" s="21"/>
       <c r="D56" s="16"/>
       <c r="E56" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G56" s="20" t="s">
-        <v>49</v>
+      <c r="G56" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="2:7">
       <c r="B57" s="16"/>
-      <c r="C57" s="23"/>
+      <c r="C57" s="21"/>
       <c r="D57" s="16"/>
       <c r="E57" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G57" s="20" t="s">
-        <v>51</v>
+      <c r="G57" s="18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="2:7">
       <c r="B58" s="16"/>
-      <c r="C58" s="23"/>
+      <c r="C58" s="21"/>
       <c r="D58" s="16"/>
       <c r="E58" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="20" t="s">
-        <v>53</v>
+      <c r="G58" s="18" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="2:7">
       <c r="B59" s="16"/>
-      <c r="C59" s="23"/>
+      <c r="C59" s="21"/>
       <c r="D59" s="16"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
-      <c r="G59" s="20"/>
+      <c r="G59" s="18"/>
     </row>
     <row r="60" spans="2:7">
       <c r="B60" s="16"/>
-      <c r="C60" s="23"/>
+      <c r="C60" s="21"/>
       <c r="D60" s="16"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
-      <c r="G60" s="20"/>
+      <c r="G60" s="18"/>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="16"/>
-      <c r="C61" s="23"/>
+      <c r="C61" s="21"/>
       <c r="D61" s="16"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
-      <c r="G61" s="20"/>
+      <c r="G61" s="18"/>
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="16"/>
-      <c r="C62" s="23"/>
+      <c r="C62" s="21"/>
       <c r="D62" s="16"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
-      <c r="G62" s="20"/>
+      <c r="G62" s="18"/>
     </row>
     <row r="63" spans="2:7">
       <c r="B63" s="16"/>
-      <c r="C63" s="23"/>
+      <c r="C63" s="21"/>
       <c r="D63" s="16"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
-      <c r="G63" s="20"/>
+      <c r="G63" s="18"/>
     </row>
     <row r="64" spans="2:7">
       <c r="B64" s="16"/>
-      <c r="C64" s="23"/>
+      <c r="C64" s="21"/>
       <c r="D64" s="16"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
-      <c r="G64" s="20"/>
+      <c r="G64" s="18"/>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="21"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="21"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="19"/>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
-      <c r="G65" s="20"/>
+      <c r="G65" s="18"/>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="1">
         <v>6</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D66" s="12">
         <v>1</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
-      <c r="G66" s="20"/>
+      <c r="G66" s="18"/>
     </row>
     <row r="67" spans="2:7">
       <c r="B67" s="12"/>
@@ -2296,7 +2304,7 @@
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
-      <c r="G67" s="20"/>
+      <c r="G67" s="18"/>
     </row>
     <row r="68" spans="2:7">
       <c r="B68" s="12"/>
@@ -2304,7 +2312,7 @@
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
-      <c r="G68" s="20"/>
+      <c r="G68" s="18"/>
     </row>
     <row r="69" spans="2:7">
       <c r="B69" s="12"/>
@@ -2312,7 +2320,7 @@
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
       <c r="F69" s="12"/>
-      <c r="G69" s="20"/>
+      <c r="G69" s="18"/>
     </row>
     <row r="70" spans="2:7">
       <c r="B70" s="12"/>
@@ -2320,7 +2328,7 @@
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
       <c r="F70" s="12"/>
-      <c r="G70" s="20"/>
+      <c r="G70" s="18"/>
     </row>
     <row r="71" spans="2:7">
       <c r="B71" s="12"/>
@@ -2328,7 +2336,7 @@
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
-      <c r="G71" s="20"/>
+      <c r="G71" s="18"/>
     </row>
     <row r="72" spans="2:7">
       <c r="B72" s="12"/>
@@ -2336,7 +2344,7 @@
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
       <c r="F72" s="12"/>
-      <c r="G72" s="20"/>
+      <c r="G72" s="18"/>
     </row>
     <row r="73" spans="2:7">
       <c r="B73" s="12"/>
@@ -2344,7 +2352,7 @@
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
-      <c r="G73" s="20"/>
+      <c r="G73" s="18"/>
     </row>
     <row r="74" spans="2:7">
       <c r="B74" s="12"/>
@@ -2352,7 +2360,7 @@
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
       <c r="F74" s="12"/>
-      <c r="G74" s="20"/>
+      <c r="G74" s="18"/>
     </row>
     <row r="75" spans="2:7">
       <c r="B75" s="12"/>
@@ -2360,7 +2368,7 @@
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
       <c r="F75" s="12"/>
-      <c r="G75" s="20"/>
+      <c r="G75" s="18"/>
     </row>
     <row r="76" spans="2:7">
       <c r="B76" s="12"/>
@@ -2368,29 +2376,29 @@
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
       <c r="F76" s="12"/>
-      <c r="G76" s="20"/>
+      <c r="G76" s="18"/>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="1">
         <v>7</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D77" s="12">
         <v>1</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F77" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G77" s="20" t="s">
-        <v>59</v>
+      <c r="G77" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="2:7">
@@ -2398,13 +2406,13 @@
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
       <c r="E78" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F78" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G78" s="20" t="s">
-        <v>61</v>
+      <c r="G78" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="2:7">
@@ -2412,13 +2420,13 @@
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
       <c r="E79" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F79" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G79" s="20" t="s">
-        <v>63</v>
+      <c r="G79" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="2:7">
@@ -2427,7 +2435,7 @@
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
       <c r="F80" s="12"/>
-      <c r="G80" s="20"/>
+      <c r="G80" s="18"/>
     </row>
     <row r="81" spans="2:7">
       <c r="B81" s="12"/>
@@ -2435,7 +2443,7 @@
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
       <c r="F81" s="12"/>
-      <c r="G81" s="20"/>
+      <c r="G81" s="18"/>
     </row>
     <row r="82" spans="2:7">
       <c r="B82" s="12"/>
@@ -2443,7 +2451,7 @@
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
       <c r="F82" s="12"/>
-      <c r="G82" s="20"/>
+      <c r="G82" s="18"/>
     </row>
     <row r="83" spans="2:7">
       <c r="B83" s="12"/>
@@ -2451,7 +2459,7 @@
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
-      <c r="G83" s="20"/>
+      <c r="G83" s="18"/>
     </row>
     <row r="84" spans="2:7">
       <c r="B84" s="12"/>
@@ -2459,7 +2467,7 @@
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
-      <c r="G84" s="20"/>
+      <c r="G84" s="18"/>
     </row>
     <row r="85" spans="2:7">
       <c r="B85" s="12"/>
@@ -2467,7 +2475,7 @@
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
-      <c r="G85" s="20"/>
+      <c r="G85" s="18"/>
     </row>
     <row r="86" spans="2:7">
       <c r="B86" s="12"/>
@@ -2475,7 +2483,7 @@
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
-      <c r="G86" s="20"/>
+      <c r="G86" s="18"/>
     </row>
     <row r="87" spans="2:7">
       <c r="B87" s="12"/>
@@ -2483,7 +2491,7 @@
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
-      <c r="G87" s="20"/>
+      <c r="G87" s="18"/>
     </row>
     <row r="88" spans="2:7">
       <c r="B88" s="12"/>
@@ -2491,7 +2499,7 @@
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
-      <c r="G88" s="20"/>
+      <c r="G88" s="18"/>
     </row>
     <row r="89" spans="2:7">
       <c r="B89" s="12"/>
@@ -2499,7 +2507,7 @@
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
       <c r="F89" s="12"/>
-      <c r="G89" s="20"/>
+      <c r="G89" s="18"/>
     </row>
     <row r="90" spans="2:7">
       <c r="B90" s="12"/>
@@ -2507,7 +2515,7 @@
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
-      <c r="G90" s="20"/>
+      <c r="G90" s="18"/>
     </row>
     <row r="91" spans="2:7">
       <c r="B91" s="12"/>
@@ -2515,29 +2523,29 @@
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
       <c r="F91" s="12"/>
-      <c r="G91" s="20"/>
+      <c r="G91" s="18"/>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="1">
         <v>8</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D92" s="12">
         <v>1</v>
       </c>
       <c r="E92" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F92" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G92" s="20" t="s">
-        <v>67</v>
+      <c r="G92" s="18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="2:7">
@@ -2546,7 +2554,7 @@
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
       <c r="F93" s="12"/>
-      <c r="G93" s="20"/>
+      <c r="G93" s="18"/>
     </row>
     <row r="94" spans="2:7">
       <c r="B94" s="12"/>
@@ -2554,7 +2562,7 @@
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
       <c r="F94" s="12"/>
-      <c r="G94" s="20"/>
+      <c r="G94" s="18"/>
     </row>
     <row r="95" spans="2:7">
       <c r="B95" s="12"/>
@@ -2562,7 +2570,7 @@
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
       <c r="F95" s="12"/>
-      <c r="G95" s="20"/>
+      <c r="G95" s="18"/>
     </row>
     <row r="96" spans="2:7">
       <c r="B96" s="12"/>
@@ -2570,7 +2578,7 @@
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
       <c r="F96" s="12"/>
-      <c r="G96" s="20"/>
+      <c r="G96" s="18"/>
     </row>
     <row r="97" spans="2:7">
       <c r="B97" s="12"/>
@@ -2578,7 +2586,7 @@
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
       <c r="F97" s="12"/>
-      <c r="G97" s="20"/>
+      <c r="G97" s="18"/>
     </row>
     <row r="98" spans="2:7">
       <c r="B98" s="12"/>
@@ -2586,7 +2594,7 @@
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
       <c r="F98" s="12"/>
-      <c r="G98" s="20"/>
+      <c r="G98" s="18"/>
     </row>
     <row r="99" spans="2:7">
       <c r="B99" s="12"/>
@@ -2594,7 +2602,7 @@
       <c r="D99" s="12"/>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
-      <c r="G99" s="20"/>
+      <c r="G99" s="18"/>
     </row>
     <row r="100" spans="2:7">
       <c r="B100" s="12"/>
@@ -2602,7 +2610,7 @@
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
       <c r="F100" s="12"/>
-      <c r="G100" s="20"/>
+      <c r="G100" s="18"/>
     </row>
     <row r="101" spans="2:7">
       <c r="B101" s="12"/>
@@ -2610,7 +2618,7 @@
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
       <c r="F101" s="12"/>
-      <c r="G101" s="20"/>
+      <c r="G101" s="18"/>
     </row>
     <row r="102" spans="2:7">
       <c r="B102" s="12"/>
@@ -2618,7 +2626,7 @@
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
-      <c r="G102" s="20"/>
+      <c r="G102" s="18"/>
     </row>
     <row r="103" spans="2:7">
       <c r="B103" s="12"/>
@@ -2626,7 +2634,7 @@
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
       <c r="F103" s="12"/>
-      <c r="G103" s="20"/>
+      <c r="G103" s="18"/>
     </row>
     <row r="104" spans="2:7">
       <c r="B104" s="12"/>
@@ -2634,7 +2642,7 @@
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
       <c r="F104" s="12"/>
-      <c r="G104" s="20"/>
+      <c r="G104" s="18"/>
     </row>
     <row r="105" spans="2:7">
       <c r="B105" s="12"/>
@@ -2642,7 +2650,7 @@
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
       <c r="F105" s="12"/>
-      <c r="G105" s="20"/>
+      <c r="G105" s="18"/>
     </row>
     <row r="106" spans="2:7">
       <c r="B106" s="12"/>
@@ -2650,7 +2658,7 @@
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
-      <c r="G106" s="20"/>
+      <c r="G106" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="33">

</xml_diff>